<commit_message>
last update => 1401/02/25
</commit_message>
<xml_diff>
--- a/WEB-PACK/124/124.xlsx
+++ b/WEB-PACK/124/124.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\124\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\WEB-PACK\124\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F566626-40A6-4923-9FDF-3E2F64754401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EA22C0-68DD-47A8-8436-0B01969E1B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -596,7 +596,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,15 +1512,15 @@
         <v>9.5</v>
       </c>
       <c r="D26" s="14">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>41.449999999999989</v>
+        <v>76.449999999999989</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>41.449999999999989</v>
+        <v>76.449999999999989</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>